<commit_message>
updated the date in config file
</commit_message>
<xml_diff>
--- a/admin/project_documents/li_bangkok_config.xlsx
+++ b/admin/project_documents/li_bangkok_config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ind_bangkok\admin\project_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\ind_lancet\admin\project_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD462BE7-0DFB-4E47-8929-42A77F256385}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0779474-D29D-4F95-B7AA-0201CE39E697}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12015" xr2:uid="{CEEBC2D6-9E16-419D-AFB3-474A6DD9A925}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12012" xr2:uid="{CEEBC2D6-9E16-419D-AFB3-474A6DD9A925}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -3840,9 +3840,6 @@
     <t xml:space="preserve">The note itself </t>
   </si>
   <si>
-    <t>Carl Higgs, 21 January 2018</t>
-  </si>
-  <si>
     <t>This worksheet provides a catalogue of project resources compiled by Carl Higgs, Amanda Alderton, and Hannah Badland in coordination with the Bangkok Metropolitan Administration, 2019</t>
   </si>
   <si>
@@ -3850,6 +3847,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Carl Higgs, 21 January 2019</t>
   </si>
 </sst>
 </file>
@@ -4773,48 +4773,48 @@
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="107.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="107.109375" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
         <v>449</v>
       </c>
       <c r="B1" s="74"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>1191</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>1192</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="77" t="s">
         <v>451</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>454</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
       <c r="B13" s="82" t="s">
         <v>38</v>
@@ -4843,7 +4843,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="82" t="s">
         <v>5</v>
@@ -4852,7 +4852,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
       <c r="B15" s="82" t="s">
         <v>893</v>
@@ -4861,7 +4861,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
       <c r="B16" s="82" t="s">
         <v>889</v>
@@ -4870,7 +4870,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
       <c r="B17" s="82" t="s">
         <v>890</v>
@@ -4879,12 +4879,12 @@
         <v>897</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="84"/>
       <c r="B18" s="85"/>
       <c r="C18" s="86"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="s">
         <v>453</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="76"/>
       <c r="B20" s="76" t="s">
         <v>381</v>
@@ -4902,7 +4902,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="76"/>
       <c r="B21" s="76" t="s">
         <v>382</v>
@@ -4911,7 +4911,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="76"/>
       <c r="B22" s="76" t="s">
         <v>238</v>
@@ -4920,7 +4920,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="76"/>
       <c r="B23" s="76" t="s">
         <v>246</v>
@@ -4929,7 +4929,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="76"/>
       <c r="B24" s="76" t="s">
         <v>251</v>
@@ -4938,7 +4938,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="76"/>
       <c r="B25" s="76" t="s">
         <v>386</v>
@@ -4947,7 +4947,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="76"/>
       <c r="B26" s="76" t="s">
         <v>224</v>
@@ -4956,7 +4956,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" s="76" t="s">
         <v>222</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="76" t="s">
         <v>221</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="76" t="s">
         <v>269</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="76" t="s">
         <v>1</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="76" t="s">
         <v>239</v>
       </c>
@@ -4996,12 +4996,12 @@
         <v>910</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="84"/>
       <c r="B32" s="85"/>
       <c r="C32" s="86"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="75" t="s">
         <v>911</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="76"/>
       <c r="B34" s="76" t="s">
         <v>1011</v>
@@ -5019,7 +5019,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="76" t="s">
         <v>1010</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="76" t="s">
         <v>1009</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="76" t="s">
         <v>560</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="76" t="s">
         <v>561</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="76" t="s">
         <v>2</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="76" t="s">
         <v>562</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="76" t="s">
         <v>3</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="76" t="s">
         <v>563</v>
       </c>
@@ -5083,12 +5083,12 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="84"/>
       <c r="B43" s="85"/>
       <c r="C43" s="86"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="75" t="s">
         <v>1179</v>
       </c>
@@ -5097,24 +5097,24 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="11" t="s">
         <v>257</v>
       </c>
       <c r="C45" s="14"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
         <v>258</v>
       </c>
       <c r="C46" s="14"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="84"/>
       <c r="B47" s="85"/>
       <c r="C47" s="86"/>
     </row>
-    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="75" t="s">
         <v>1181</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B49" s="76" t="s">
         <v>68</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
         <v>69</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B51" s="11" t="s">
         <v>70</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" s="11" t="s">
         <v>71</v>
       </c>
@@ -5155,12 +5155,12 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="84"/>
       <c r="B53" s="85"/>
       <c r="C53" s="86"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="75" t="s">
         <v>1</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B55" s="76" t="s">
         <v>226</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B56" s="14" t="s">
         <v>228</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" s="11" t="s">
         <v>227</v>
       </c>
@@ -5213,18 +5213,18 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="18" customWidth="1"/>
     <col min="3" max="3" width="56" style="18" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
-    <col min="5" max="51" width="3.85546875" style="5" customWidth="1"/>
-    <col min="52" max="52" width="83.5703125" style="18" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="51" width="3.88671875" style="5" customWidth="1"/>
+    <col min="52" max="52" width="83.5546875" style="18" customWidth="1"/>
+    <col min="53" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
@@ -5288,7 +5288,7 @@
       <c r="AY1" s="102"/>
       <c r="AZ1" s="29"/>
     </row>
-    <row r="2" spans="1:52" s="27" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" s="27" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -5438,7 +5438,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="3" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>39</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="4" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>456</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
         <v>456</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="6" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>39</v>
       </c>
@@ -5710,13 +5710,13 @@
       <c r="AW6" s="36"/>
       <c r="AX6" s="36"/>
       <c r="AY6" s="72" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="AZ6" s="37" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="7" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
         <v>456</v>
       </c>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="AZ7" s="37"/>
     </row>
-    <row r="8" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>456</v>
       </c>
@@ -5848,7 +5848,7 @@
       </c>
       <c r="AZ8" s="37"/>
     </row>
-    <row r="9" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>456</v>
       </c>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="AZ9" s="37"/>
     </row>
-    <row r="10" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>39</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>39</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="12" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>39</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="13" spans="1:52" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>39</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="14" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
         <v>456</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="15" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>456</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>39</v>
       </c>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="AZ16" s="37"/>
     </row>
-    <row r="17" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>456</v>
       </c>
@@ -6492,7 +6492,7 @@
       </c>
       <c r="AZ17" s="37"/>
     </row>
-    <row r="18" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>39</v>
       </c>
@@ -6568,7 +6568,7 @@
       </c>
       <c r="AZ18" s="37"/>
     </row>
-    <row r="19" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>39</v>
       </c>
@@ -6644,7 +6644,7 @@
       </c>
       <c r="AZ19" s="37"/>
     </row>
-    <row r="20" spans="1:52" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" s="33" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>39</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
         <v>39</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="22" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>40</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="23" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>40</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="24" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>456</v>
       </c>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="AZ24" s="37"/>
     </row>
-    <row r="25" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>456</v>
       </c>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="AZ25" s="37"/>
     </row>
-    <row r="26" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>40</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
         <v>40</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:52" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>40</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="29" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>40</v>
       </c>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="AZ29" s="37"/>
     </row>
-    <row r="30" spans="1:52" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" s="33" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>40</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="31" spans="1:52" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>40</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="32" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>40</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="33" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
         <v>40</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="34" spans="1:52" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" s="33" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A34" s="30" t="s">
         <v>40</v>
       </c>
@@ -7684,7 +7684,7 @@
       </c>
       <c r="AZ34" s="37"/>
     </row>
-    <row r="35" spans="1:52" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" s="33" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>41</v>
       </c>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="AZ35" s="37"/>
     </row>
-    <row r="36" spans="1:52" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" s="33" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>41</v>
       </c>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="AZ36" s="37"/>
     </row>
-    <row r="37" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="AZ37" s="37"/>
     </row>
-    <row r="38" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>41</v>
       </c>
@@ -7996,7 +7996,7 @@
       </c>
       <c r="AZ38" s="37"/>
     </row>
-    <row r="39" spans="1:52" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
         <v>41</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="40" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="30" t="s">
         <v>41</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="41" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
         <v>41</v>
       </c>
@@ -8200,7 +8200,7 @@
       </c>
       <c r="AZ41" s="37"/>
     </row>
-    <row r="42" spans="1:52" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="30" t="s">
         <v>41</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="43" spans="1:52" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>41</v>
       </c>
@@ -8362,7 +8362,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="44" spans="1:52" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>41</v>
       </c>
@@ -8438,7 +8438,7 @@
       </c>
       <c r="AZ44" s="37"/>
     </row>
-    <row r="45" spans="1:52" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" s="33" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A45" s="30" t="s">
         <v>41</v>
       </c>
@@ -8502,7 +8502,7 @@
       <c r="AY45" s="72"/>
       <c r="AZ45" s="37"/>
     </row>
-    <row r="46" spans="1:52" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" s="33" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A46" s="30" t="s">
         <v>456</v>
       </c>
@@ -8604,21 +8604,21 @@
       <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="89" customWidth="1"/>
-    <col min="3" max="3" width="103.85546875" customWidth="1"/>
-    <col min="4" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="103.88671875" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="49.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" customWidth="1"/>
+    <col min="11" max="11" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>381</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>365</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>545</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>364</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>367</v>
       </c>
@@ -8799,7 +8799,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>244</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>243</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>245</v>
       </c>
@@ -8889,7 +8889,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>544</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>513</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>256</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>423</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>279</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>527</v>
       </c>
@@ -9069,7 +9069,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>284</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>526</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>286</v>
       </c>
@@ -9159,7 +9159,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>287</v>
       </c>
@@ -9188,7 +9188,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>288</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>289</v>
       </c>
@@ -9246,7 +9246,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>290</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>525</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>292</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>293</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>294</v>
       </c>
@@ -9394,7 +9394,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>295</v>
       </c>
@@ -9423,7 +9423,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>524</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>297</v>
       </c>
@@ -9484,7 +9484,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>298</v>
       </c>
@@ -9513,7 +9513,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>299</v>
       </c>
@@ -9542,7 +9542,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>300</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>301</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>302</v>
       </c>
@@ -9629,7 +9629,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>303</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>304</v>
       </c>
@@ -9687,7 +9687,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>335</v>
       </c>
@@ -9716,7 +9716,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>336</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>337</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>338</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>551</v>
       </c>
@@ -9835,7 +9835,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>342</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>383</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>546</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>384</v>
       </c>
@@ -9969,7 +9969,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>547</v>
       </c>
@@ -10004,7 +10004,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>523</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>522</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>387</v>
       </c>
@@ -10094,7 +10094,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>393</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>399</v>
       </c>
@@ -10164,7 +10164,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>411</v>
       </c>
@@ -10202,7 +10202,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>412</v>
       </c>
@@ -10240,7 +10240,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>541</v>
       </c>
@@ -10266,7 +10266,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>543</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>539</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>439</v>
       </c>
@@ -10344,7 +10344,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>518</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>514</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>519</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>515</v>
       </c>
@@ -10427,7 +10427,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>528</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>529</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>530</v>
       </c>
@@ -10529,7 +10529,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>531</v>
       </c>
@@ -10561,18 +10561,18 @@
         <v>482</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="23" t="s">
         <v>486</v>
       </c>
       <c r="D65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="23" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>532</v>
       </c>
@@ -10604,7 +10604,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>537</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>516</v>
       </c>
@@ -10662,7 +10662,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>520</v>
       </c>
@@ -10697,7 +10697,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>517</v>
       </c>
@@ -10720,7 +10720,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>521</v>
       </c>
@@ -10755,14 +10755,14 @@
         <v>496</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="23" t="s">
         <v>501</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="22"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>538</v>
       </c>
@@ -10797,7 +10797,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>504</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>512</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>511</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>510</v>
       </c>
@@ -10925,18 +10925,18 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="19" customWidth="1"/>
-    <col min="2" max="3" width="76.5703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="5" customWidth="1"/>
-    <col min="5" max="7" width="17.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="53.28515625" style="101" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="16.5546875" style="19" customWidth="1"/>
+    <col min="2" max="3" width="76.5546875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="5" customWidth="1"/>
+    <col min="5" max="7" width="17.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="53.33203125" style="101" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>557</v>
       </c>
@@ -10946,7 +10946,7 @@
       <c r="H1" s="87"/>
       <c r="I1" s="42"/>
     </row>
-    <row r="2" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>377</v>
       </c>
@@ -10959,7 +10959,7 @@
       <c r="H2" s="87"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>378</v>
       </c>
@@ -10972,7 +10972,7 @@
       <c r="H3" s="87"/>
       <c r="I3" s="42"/>
     </row>
-    <row r="4" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>558</v>
       </c>
@@ -10983,7 +10983,7 @@
       <c r="H4" s="87"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>559</v>
       </c>
@@ -10994,7 +10994,7 @@
       <c r="H5" s="87"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
@@ -11002,7 +11002,7 @@
       <c r="H6" s="87"/>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="42"/>
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
@@ -11010,7 +11010,7 @@
       <c r="H7" s="87"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
         <v>1011</v>
       </c>
@@ -11039,7 +11039,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>564</v>
       </c>
@@ -11065,7 +11065,7 @@
       </c>
       <c r="J9" s="48"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
         <v>564</v>
       </c>
@@ -11095,7 +11095,7 @@
       </c>
       <c r="J10" s="48"/>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
         <v>564</v>
       </c>
@@ -11125,7 +11125,7 @@
       </c>
       <c r="J11" s="48"/>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
         <v>564</v>
       </c>
@@ -11155,7 +11155,7 @@
       </c>
       <c r="J12" s="48"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="46" t="s">
         <v>564</v>
       </c>
@@ -11185,7 +11185,7 @@
       </c>
       <c r="J13" s="48"/>
     </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
         <v>564</v>
       </c>
@@ -11215,7 +11215,7 @@
       </c>
       <c r="J14" s="48"/>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="46" t="s">
         <v>564</v>
       </c>
@@ -11245,7 +11245,7 @@
       </c>
       <c r="J15" s="48"/>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
         <v>564</v>
       </c>
@@ -11275,7 +11275,7 @@
       </c>
       <c r="J16" s="48"/>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>564</v>
       </c>
@@ -11305,7 +11305,7 @@
       </c>
       <c r="J17" s="48"/>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
         <v>564</v>
       </c>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="J18" s="48"/>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>564</v>
       </c>
@@ -11365,7 +11365,7 @@
       </c>
       <c r="J19" s="48"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
         <v>564</v>
       </c>
@@ -11395,7 +11395,7 @@
       </c>
       <c r="J20" s="48"/>
     </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>564</v>
       </c>
@@ -11425,7 +11425,7 @@
       </c>
       <c r="J21" s="48"/>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
         <v>564</v>
       </c>
@@ -11455,7 +11455,7 @@
       </c>
       <c r="J22" s="48"/>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
         <v>564</v>
       </c>
@@ -11485,7 +11485,7 @@
       </c>
       <c r="J23" s="48"/>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="51" t="s">
         <v>623</v>
       </c>
@@ -11515,7 +11515,7 @@
       </c>
       <c r="J24" s="48"/>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53" t="s">
         <v>623</v>
       </c>
@@ -11545,7 +11545,7 @@
       </c>
       <c r="J25" s="48"/>
     </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="51" t="s">
         <v>623</v>
       </c>
@@ -11575,7 +11575,7 @@
       </c>
       <c r="J26" s="48"/>
     </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
         <v>623</v>
       </c>
@@ -11605,7 +11605,7 @@
       </c>
       <c r="J27" s="48"/>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="51" t="s">
         <v>623</v>
       </c>
@@ -11635,7 +11635,7 @@
       </c>
       <c r="J28" s="48"/>
     </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="53" t="s">
         <v>623</v>
       </c>
@@ -11665,7 +11665,7 @@
       </c>
       <c r="J29" s="48"/>
     </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="51" t="s">
         <v>623</v>
       </c>
@@ -11695,7 +11695,7 @@
       </c>
       <c r="J30" s="48"/>
     </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="53" t="s">
         <v>623</v>
       </c>
@@ -11725,7 +11725,7 @@
       </c>
       <c r="J31" s="48"/>
     </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="51" t="s">
         <v>623</v>
       </c>
@@ -11755,7 +11755,7 @@
       </c>
       <c r="J32" s="48"/>
     </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>623</v>
       </c>
@@ -11785,7 +11785,7 @@
       </c>
       <c r="J33" s="48"/>
     </row>
-    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="51" t="s">
         <v>623</v>
       </c>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="J34" s="48"/>
     </row>
-    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="53" t="s">
         <v>623</v>
       </c>
@@ -11845,7 +11845,7 @@
       </c>
       <c r="J35" s="48"/>
     </row>
-    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="51" t="s">
         <v>623</v>
       </c>
@@ -11875,7 +11875,7 @@
       </c>
       <c r="J36" s="48"/>
     </row>
-    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="53" t="s">
         <v>623</v>
       </c>
@@ -11905,7 +11905,7 @@
       </c>
       <c r="J37" s="48"/>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="49" t="s">
         <v>623</v>
       </c>
@@ -11935,7 +11935,7 @@
       </c>
       <c r="J38" s="48"/>
     </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="53" t="s">
         <v>623</v>
       </c>
@@ -11965,7 +11965,7 @@
       </c>
       <c r="J39" s="48"/>
     </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="49" t="s">
         <v>623</v>
       </c>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="J40" s="48"/>
     </row>
-    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="53" t="s">
         <v>623</v>
       </c>
@@ -12025,7 +12025,7 @@
       </c>
       <c r="J41" s="48"/>
     </row>
-    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="49" t="s">
         <v>623</v>
       </c>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="J42" s="48"/>
     </row>
-    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="55" t="s">
         <v>51</v>
       </c>
@@ -12085,7 +12085,7 @@
       </c>
       <c r="J43" s="48"/>
     </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
         <v>51</v>
       </c>
@@ -12115,7 +12115,7 @@
       </c>
       <c r="J44" s="48"/>
     </row>
-    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="55" t="s">
         <v>51</v>
       </c>
@@ -12145,7 +12145,7 @@
       </c>
       <c r="J45" s="48"/>
     </row>
-    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="51" t="s">
         <v>51</v>
       </c>
@@ -12175,7 +12175,7 @@
       </c>
       <c r="J46" s="48"/>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="55" t="s">
         <v>51</v>
       </c>
@@ -12205,7 +12205,7 @@
       </c>
       <c r="J47" s="48"/>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="51" t="s">
         <v>51</v>
       </c>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="J48" s="48"/>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="55" t="s">
         <v>51</v>
       </c>
@@ -12265,7 +12265,7 @@
       </c>
       <c r="J49" s="48"/>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="51" t="s">
         <v>51</v>
       </c>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="J50" s="48"/>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="55" t="s">
         <v>51</v>
       </c>
@@ -12325,7 +12325,7 @@
       </c>
       <c r="J51" s="48"/>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="49" t="s">
         <v>51</v>
       </c>
@@ -12355,7 +12355,7 @@
       </c>
       <c r="J52" s="48"/>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="55" t="s">
         <v>51</v>
       </c>
@@ -12385,7 +12385,7 @@
       </c>
       <c r="J53" s="48"/>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="49" t="s">
         <v>51</v>
       </c>
@@ -12415,7 +12415,7 @@
       </c>
       <c r="J54" s="48"/>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="55" t="s">
         <v>51</v>
       </c>
@@ -12445,7 +12445,7 @@
       </c>
       <c r="J55" s="48"/>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="49" t="s">
         <v>51</v>
       </c>
@@ -12475,7 +12475,7 @@
       </c>
       <c r="J56" s="48"/>
     </row>
-    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="55" t="s">
         <v>51</v>
       </c>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="J57" s="48"/>
     </row>
-    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="49" t="s">
         <v>51</v>
       </c>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="J58" s="48"/>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="55" t="s">
         <v>51</v>
       </c>
@@ -12565,7 +12565,7 @@
       </c>
       <c r="J59" s="48"/>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="49" t="s">
         <v>51</v>
       </c>
@@ -12595,7 +12595,7 @@
       </c>
       <c r="J60" s="48"/>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="55" t="s">
         <v>51</v>
       </c>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="J61" s="48"/>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="49" t="s">
         <v>51</v>
       </c>
@@ -12655,7 +12655,7 @@
       </c>
       <c r="J62" s="48"/>
     </row>
-    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="55" t="s">
         <v>51</v>
       </c>
@@ -12685,7 +12685,7 @@
       </c>
       <c r="J63" s="48"/>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="51" t="s">
         <v>763</v>
       </c>
@@ -12715,7 +12715,7 @@
       </c>
       <c r="J64" s="48"/>
     </row>
-    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="58" t="s">
         <v>763</v>
       </c>
@@ -12745,7 +12745,7 @@
       </c>
       <c r="J65" s="48"/>
     </row>
-    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="51" t="s">
         <v>763</v>
       </c>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="J66" s="48"/>
     </row>
-    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
         <v>763</v>
       </c>
@@ -12805,7 +12805,7 @@
       </c>
       <c r="J67" s="48"/>
     </row>
-    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="51" t="s">
         <v>763</v>
       </c>
@@ -12835,7 +12835,7 @@
       </c>
       <c r="J68" s="48"/>
     </row>
-    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="s">
         <v>763</v>
       </c>
@@ -12865,7 +12865,7 @@
       </c>
       <c r="J69" s="48"/>
     </row>
-    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="51" t="s">
         <v>763</v>
       </c>
@@ -12892,7 +12892,7 @@
       </c>
       <c r="I70" s="52"/>
     </row>
-    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="58" t="s">
         <v>763</v>
       </c>
@@ -12922,7 +12922,7 @@
       </c>
       <c r="J71" s="48"/>
     </row>
-    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="60" t="s">
         <v>787</v>
       </c>
@@ -12952,7 +12952,7 @@
       </c>
       <c r="J72" s="48"/>
     </row>
-    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="51" t="s">
         <v>787</v>
       </c>
@@ -12982,7 +12982,7 @@
       </c>
       <c r="J73" s="48"/>
     </row>
-    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="60" t="s">
         <v>787</v>
       </c>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="J74" s="48"/>
     </row>
-    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="51" t="s">
         <v>787</v>
       </c>
@@ -13042,7 +13042,7 @@
       </c>
       <c r="J75" s="48"/>
     </row>
-    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="60" t="s">
         <v>787</v>
       </c>
@@ -13072,7 +13072,7 @@
       </c>
       <c r="J76" s="48"/>
     </row>
-    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="51" t="s">
         <v>787</v>
       </c>
@@ -13102,7 +13102,7 @@
       </c>
       <c r="J77" s="48"/>
     </row>
-    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="60" t="s">
         <v>787</v>
       </c>
@@ -13132,7 +13132,7 @@
       </c>
       <c r="J78" s="48"/>
     </row>
-    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="51" t="s">
         <v>787</v>
       </c>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="J79" s="48"/>
     </row>
-    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="63" t="s">
         <v>817</v>
       </c>
@@ -13192,7 +13192,7 @@
       </c>
       <c r="J80" s="48"/>
     </row>
-    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="51" t="s">
         <v>817</v>
       </c>
@@ -13222,7 +13222,7 @@
       </c>
       <c r="J81" s="48"/>
     </row>
-    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="63" t="s">
         <v>817</v>
       </c>
@@ -13252,7 +13252,7 @@
       </c>
       <c r="J82" s="48"/>
     </row>
-    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="51" t="s">
         <v>817</v>
       </c>
@@ -13282,7 +13282,7 @@
       </c>
       <c r="J83" s="48"/>
     </row>
-    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="63" t="s">
         <v>817</v>
       </c>
@@ -13312,7 +13312,7 @@
       </c>
       <c r="J84" s="48"/>
     </row>
-    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="51" t="s">
         <v>817</v>
       </c>
@@ -13342,7 +13342,7 @@
       </c>
       <c r="J85" s="48"/>
     </row>
-    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="63" t="s">
         <v>817</v>
       </c>
@@ -13372,7 +13372,7 @@
       </c>
       <c r="J86" s="48"/>
     </row>
-    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="51" t="s">
         <v>817</v>
       </c>
@@ -13402,7 +13402,7 @@
       </c>
       <c r="J87" s="48"/>
     </row>
-    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="65" t="s">
         <v>840</v>
       </c>
@@ -13432,7 +13432,7 @@
       </c>
       <c r="J88" s="48"/>
     </row>
-    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="51" t="s">
         <v>840</v>
       </c>
@@ -13462,7 +13462,7 @@
       </c>
       <c r="J89" s="48"/>
     </row>
-    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="65" t="s">
         <v>840</v>
       </c>
@@ -13492,7 +13492,7 @@
       </c>
       <c r="J90" s="48"/>
     </row>
-    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="51" t="s">
         <v>840</v>
       </c>
@@ -13522,7 +13522,7 @@
       </c>
       <c r="J91" s="48"/>
     </row>
-    <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="65" t="s">
         <v>840</v>
       </c>
@@ -13552,7 +13552,7 @@
       </c>
       <c r="J92" s="48"/>
     </row>
-    <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="49" t="s">
         <v>840</v>
       </c>
@@ -13582,7 +13582,7 @@
       </c>
       <c r="J93" s="48"/>
     </row>
-    <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="65" t="s">
         <v>840</v>
       </c>
@@ -13612,7 +13612,7 @@
       </c>
       <c r="J94" s="48"/>
     </row>
-    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="67" t="s">
         <v>861</v>
       </c>
@@ -13642,7 +13642,7 @@
       </c>
       <c r="J95" s="48"/>
     </row>
-    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="51" t="s">
         <v>861</v>
       </c>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="J96" s="48"/>
     </row>
-    <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="67" t="s">
         <v>861</v>
       </c>
@@ -13702,7 +13702,7 @@
       </c>
       <c r="J97" s="48"/>
     </row>
-    <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="51" t="s">
         <v>861</v>
       </c>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="J98" s="48"/>
     </row>
-    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="67" t="s">
         <v>861</v>
       </c>
@@ -13762,7 +13762,7 @@
       </c>
       <c r="J99" s="48"/>
     </row>
-    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="51" t="s">
         <v>861</v>
       </c>
@@ -13790,7 +13790,7 @@
       </c>
       <c r="J100" s="48"/>
     </row>
-    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="67" t="s">
         <v>861</v>
       </c>
@@ -13818,7 +13818,7 @@
       </c>
       <c r="J101" s="48"/>
     </row>
-    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="69" t="s">
         <v>861</v>
       </c>
@@ -13861,13 +13861,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="95.7109375" customWidth="1"/>
+    <col min="2" max="2" width="95.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>257</v>
       </c>
@@ -13875,7 +13875,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>535</v>
       </c>
@@ -13883,7 +13883,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>533</v>
       </c>
@@ -13891,7 +13891,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>405</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>542</v>
       </c>
@@ -13907,7 +13907,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>480</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>261</v>
       </c>
@@ -13923,7 +13923,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>259</v>
       </c>
@@ -13931,7 +13931,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -13939,7 +13939,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>264</v>
       </c>
@@ -13947,7 +13947,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>235</v>
       </c>
@@ -13955,7 +13955,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>266</v>
       </c>
@@ -13963,7 +13963,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>548</v>
       </c>
@@ -13971,7 +13971,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -13979,7 +13979,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>478</v>
       </c>
@@ -13987,7 +13987,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>404</v>
       </c>
@@ -14014,15 +14014,15 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="54.5546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>68</v>
       </c>
@@ -14036,7 +14036,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -14064,7 +14064,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -14092,7 +14092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -14148,7 +14148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -14162,7 +14162,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -14176,7 +14176,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -14190,7 +14190,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -14218,7 +14218,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -14232,7 +14232,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -14260,7 +14260,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -14274,7 +14274,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -14288,7 +14288,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -14302,7 +14302,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -14316,7 +14316,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -14327,7 +14327,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -14338,7 +14338,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -14349,7 +14349,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -14360,7 +14360,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>218</v>
       </c>
@@ -14371,7 +14371,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>131</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -14390,7 +14390,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -14401,7 +14401,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -14412,7 +14412,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -14423,7 +14423,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>206</v>
       </c>
@@ -14448,7 +14448,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>207</v>
       </c>
@@ -14459,7 +14459,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>208</v>
       </c>
@@ -14470,7 +14470,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>209</v>
       </c>
@@ -14481,7 +14481,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>210</v>
       </c>
@@ -14492,7 +14492,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>211</v>
       </c>
@@ -14503,7 +14503,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -14514,7 +14514,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -14528,7 +14528,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>153</v>
       </c>
@@ -14567,7 +14567,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -14581,7 +14581,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -14595,7 +14595,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>160</v>
       </c>
@@ -14609,7 +14609,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -14623,7 +14623,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>166</v>
       </c>
@@ -14637,7 +14637,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -14651,7 +14651,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>171</v>
       </c>
@@ -14665,7 +14665,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>173</v>
       </c>
@@ -14679,7 +14679,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -14693,7 +14693,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -14707,7 +14707,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -14721,7 +14721,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>182</v>
       </c>
@@ -14735,7 +14735,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>185</v>
       </c>
@@ -14749,7 +14749,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>188</v>
       </c>
@@ -14763,7 +14763,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>191</v>
       </c>
@@ -14777,7 +14777,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>194</v>
       </c>
@@ -14791,7 +14791,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>196</v>
       </c>
@@ -14805,7 +14805,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>199</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>201</v>
       </c>
@@ -14827,7 +14827,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>203</v>
       </c>
@@ -14855,13 +14855,13 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13"/>
+    <col min="1" max="2" width="9.109375" style="13"/>
     <col min="3" max="3" width="71" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>226</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>20181130</v>
       </c>
@@ -14883,7 +14883,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>20181211</v>
       </c>
@@ -14894,7 +14894,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>20181211</v>
       </c>

</xml_diff>